<commit_message>
basic file searching finished
</commit_message>
<xml_diff>
--- a/cli/report.xlsx
+++ b/cli/report.xlsx
@@ -1,56 +1,324 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2326796F-9284-421F-94A2-02588E57D364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Report" state="visible" r:id="rId4"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>lastModified</t>
-  </si>
-  <si>
-    <t>refIndex</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
-    <t>DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\tiedemann\Messe Berlin GmbH\Event Services - ES-Veranstaltungsproduktion\DROID\DROID 25\009_Reinigung und Entsorgung\Kalkulation\DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx</t>
-  </si>
-  <si>
-    <t>DROID 25_KALK_SASSE_Reinigung_RT_20250522.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\tiedemann\Messe Berlin GmbH\Event Services - ES-Veranstaltungsproduktion\DROID\DROID 25\009_Reinigung und Entsorgung\Kalkulation\DROID 25_KALK_SASSE_Reinigung_RT_20250522.xlsx</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>FUNK</t>
+  </si>
+  <si>
+    <t>[{"name":"FUNK25_CWS_SFM-Bestellüberischt_DG_20250828.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\Schmutzfangmatten\\FUNK25_CWS_SFM-Bestellüberischt_DG_20250828.xlsx","lastModified":"2025-09-15T07:16:31.000Z","refIndex":41982,"score":0.000006128646825844065},{"name":"NL_IFA2025_Abrechnungslayout_Master.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\NL_IFA2025_Abrechnungslayout_Master.xlsx","lastModified":"2025-09-19T05:48:41.835Z","refIndex":41996,"score":0.000006128646825844065},{"name":"NL_IFA2025_Abrechnungslayout_MediaDays.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\NL_IFA2025_Abrechnungslayout_MediaDays.xlsx","lastModified":"2025-09-24T09:10:10.000Z","refIndex":41997,"score":0.000006128646825844065},{"name":"NL_IFA2025_Abrechnungslayout_Showstoppers.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\NL_IFA2025_Abrechnungslayout_Showstoppers.xlsx","lastModified":"2025-09-24T09:05:48.000Z","refIndex":41998,"score":0.000006128646825844065},{"name":"FUNK25_China-Brand-Night_MSH_KAL_SASSE_REINIGUNG_NK_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Abrechnung\\FUNK25_China-Brand-Night_MSH_KAL_SASSE_REINIGUNG_NK_20250926.xlsx","lastModified":"2025-09-30T06:14:10.000Z","refIndex":42001,"score":0.000006128646825844065},{"name":"FUNK25_H12_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Abrechnung\\FUNK25_H12_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","lastModified":"2025-09-30T06:09:11.000Z","refIndex":42003,"score":0.000006128646825844065},{"name":"FUNK25_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Abrechnung\\FUNK25_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","lastModified":"2025-09-30T06:09:12.000Z","refIndex":42004,"score":0.000006128646825844065},{"name":"FUNK25_MediaDays_BECC_Sasse_Reinigung_NK_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Abrechnung\\FUNK25_MediaDays_BECC_Sasse_Reinigung_NK_20250926.xlsx","lastModified":"2025-09-30T06:09:12.000Z","refIndex":42005,"score":0.000006128646825844065},{"name":"FUNK_EÖ25_CCB_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Abrechnung\\FUNK_EÖ25_CCB_KALK_SASSE_REINIGUNG_NK_20250926.xlsx","lastModified":"2025-09-30T06:09:11.000Z","refIndex":42008,"score":0.000006128646825844065},{"name":"FUNK25_KALK_SASSE_REINIGUNG_RW_20250917.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Hauptlayout\\FUNK25_KALK_SASSE_REINIGUNG_RW_20250917.xlsx","lastModified":"2025-09-30T06:13:13.000Z","refIndex":42011,"score":0.000006128646825844065},{"name":"FUNK25_BECC_ABR_WISAG_Master_Reinigung_JU_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_BECC_ABR_WISAG_Master_Reinigung_JU_20251001.xlsx","lastModified":"2025-10-06T09:34:41.000Z","refIndex":42015,"score":0.000006128646825844065},{"name":"FUNK25_BECC_KAL_WISAG_Master_Reinigung_JI_20251006.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_BECC_KAL_WISAG_Master_Reinigung_JI_20251006.xlsx","lastModified":"2025-10-06T09:38:33.000Z","refIndex":42016,"score":0.000006128646825844065},{"name":"FUNK25_Global-Markets_BECC_ABR_WISAG_Reinigung_JU_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_Global-Markets_BECC_ABR_WISAG_Reinigung_JU_20251001.xlsx","lastModified":"2025-10-01T12:48:38.000Z","refIndex":42017,"score":0.000006128646825844065},{"name":"FUNK25_Global-Markets_BECC_KAL_WISAG_Reinigung_JI_20251006.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_Global-Markets_BECC_KAL_WISAG_Reinigung_JI_20251006.xlsx","lastModified":"2025-10-06T09:43:47.000Z","refIndex":42018,"score":0.000006128646825844065},{"name":"FUNK25_MediaDays_BECC_ABR_WISAG_Reinigung_JU_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_MediaDays_BECC_ABR_WISAG_Reinigung_JU_20251001.xlsx","lastModified":"2025-10-01T12:48:38.000Z","refIndex":42019,"score":0.000006128646825844065},{"name":"FUNK25_MediaDays_BECC_KAL_WISAG_Reinigung_JI_20250831.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_MediaDays_BECC_KAL_WISAG_Reinigung_JI_20250831.xlsx","lastModified":"2025-10-06T09:48:11.000Z","refIndex":42020,"score":0.000006128646825844065},{"name":"FUNK25_SOG_ABR_WISAG_Reinigung_JU_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_SOG_ABR_WISAG_Reinigung_JU_20251001.xlsx","lastModified":"2025-10-01T12:48:38.000Z","refIndex":42021,"score":0.000006128646825844065},{"name":"FUNK25_SOG_KAL_WISAG_Reinigung_JI_20250903.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\FUNK25_SOG_KAL_WISAG_Reinigung_JI_20250903.xlsx","lastModified":"2025-09-07T16:04:16.000Z","refIndex":42022,"score":0.000006128646825844065},{"name":"FUNK25_BECC_KAL_WISAG_Glas-Reinigung_RW_20250826.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG-Glas\\FUNK25_BECC_KAL_WISAG_Glas-Reinigung_RW_20250826.xlsx","lastModified":"2025-09-07T15:07:37.000Z","refIndex":42023,"score":0.000006128646825844065},{"name":"FUNK 25_BECC_ABR_ALBA_Entsorgung_DG_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\FUNK 25_BECC_ABR_ALBA_Entsorgung_DG_20250930.xlsx","lastModified":"2025-09-25T09:32:21.000Z","refIndex":41973,"score":0.00001131032569734829},{"name":"FUNK 25_BECC_KALK_ALBA_Entsorgung_RT_20250822.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\FUNK 25_BECC_KALK_ALBA_Entsorgung_RT_20250822.xlsx","lastModified":"2025-09-05T10:44:37.000Z","refIndex":41975,"score":0.00001131032569734829},{"name":"FUNK 25_CWS_Ladycarebehälter_Master_DG_20250724.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\Hygieneboxen\\FUNK 25_CWS_Ladycarebehälter_Master_DG_20250724.xlsx","lastModified":"2025-08-22T13:42:07.155Z","refIndex":41976,"score":0.00001131032569734829},{"name":"FUNK 25_WC-Planung_Master_DG_20250730.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\Hygieneboxen\\FUNK 25_WC-Planung_Master_DG_20250730.xlsx","lastModified":"2025-08-22T09:11:14.000Z","refIndex":41978,"score":0.00001131032569734829},{"name":"FUNK 25_KALK_NL_MediaDays_JI_20250831.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_MediaDays_JI_20250831.xlsx","lastModified":"2025-09-01T06:42:41.282Z","refIndex":41985,"score":0.00001131032569734829},{"name":"FUNK 25_KALK_NL_Reinigung_MASTER_DG_20250708.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_Reinigung_MASTER_DG_20250708.xlsx","lastModified":"2025-09-17T06:55:30.000Z","refIndex":41987,"score":0.00001131032569734829},{"name":"FUNK 25_KALK_NL_Showstoppers_RT_20250717.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_Showstoppers_RT_20250717.xlsx","lastModified":"2025-10-06T10:05:08.000Z","refIndex":41988,"score":0.00001131032569734829},{"name":"NL_IFA2025_Abrechnungslayout_Cheari Award.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\NL_IFA2025_Abrechnungslayout_Cheari Award.xlsx","lastModified":"2025-09-24T09:06:54.000Z","refIndex":41994,"score":0.00001131032569734829},{"name":"FUNK25_MediaDays_BECC_Sasse_Reinigung_RW_20250906.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Media Days\\FUNK25_MediaDays_BECC_Sasse_Reinigung_RW_20250906.xlsx","lastModified":"2025-09-26T08:19:15.000Z","refIndex":42014,"score":0.00001131032569734829},{"name":"FUNK25_BECC_KAL_WISAG_Master_Reinigung_JI_2025020.xlsx.lnk","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\MBPro\\Dev\\WISAG Haupt-VA\\FUNK25_BECC_KAL_WISAG_Master_Reinigung_JI_2025020.xlsx.lnk","lastModified":"2025-08-20T04:59:37.000Z","refIndex":42028,"score":0.00001131032569734829},{"name":"FUNK 25_BECC_KALK_ALBA_Entsorgung SOG_RT_20250822.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\FUNK 25_BECC_KALK_ALBA_Entsorgung SOG_RT_20250822.xlsx","lastModified":"2025-08-22T13:51:28.000Z","refIndex":41974,"score":0.000018733759825364087},{"name":"FUNK 25_KALK_NL_Cheari Award_RT_20250703.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_Cheari Award_RT_20250703.xlsx","lastModified":"2025-09-04T06:29:20.000Z","refIndex":41983,"score":0.000018733759825364087},{"name":"NL_IFA2025_Abrechnungslayout_GFK NIQ Präsentation.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\NL_IFA2025_Abrechnungslayout_GFK NIQ Präsentation.xlsx","lastModified":"2025-09-24T09:08:34.000Z","refIndex":41995,"score":0.000018733759825364087},{"name":"FUNK25_China-Brand-Night_MSH_KAL_SASSE_REINIGUNG_JI_20250819.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\China Brand Night\\FUNK25_China-Brand-Night_MSH_KAL_SASSE_REINIGUNG_JI_20250819.xlsx","lastModified":"2025-09-30T06:13:51.000Z","refIndex":42009,"score":0.000018733759825364087},{"name":"FUNK25_CWS_SFM-Bestellüberischt_DG_20250828.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\MBPro\\Dev\\CWS Schmutzfangmatten Haupt-VA\\FUNK25_CWS_SFM-Bestellüberischt_DG_20250828.xlsx.url","lastModified":"2025-07-29T13:44:42.000Z","refIndex":42026,"score":0.000018733759825364087},{"name":"IFA NEXT 2025_Pre-built_22082028.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Veranstaltungsinfo\\IFA NEXT 2025_Pre-built_22082028.xlsx","lastModified":"2025-08-28T06:28:38.000Z","refIndex":42047,"score":0.000018733759825364087},{"name":"FUNK 25_KALK_NL_GFK NIQ Präsentation_RT_20250717.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_GFK NIQ Präsentation_RT_20250717.xlsx","lastModified":"2025-09-04T06:29:21.000Z","refIndex":41984,"score":0.000029930999877580322},{"name":"FUNK_EÖ25_CCB_KALK_SASSE_REINIGUNG_RW_20250829.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\EÖ (CCB Halle A)\\FUNK_EÖ25_CCB_KALK_SASSE_REINIGUNG_RW_20250829.xlsx","lastModified":"2025-09-26T08:18:56.000Z","refIndex":42010,"score":0.000029930999877580322},{"name":"FUNK 25_CWS_Ladycarebehälter_Master_DG_20250724.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\MBPro\\Dev\\CWS Ladycare Haupt-VA\\FUNK 25_CWS_Ladycarebehälter_Master_DG_20250724.xlsx.url","lastModified":"2025-07-29T13:36:27.000Z","refIndex":42024,"score":0.000029930999877580322},{"name":"FUNK 25_KALK_NL_Reinigung_MASTER_DG_20250708.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\MBPro\\Dev\\New Line Haupt-VA\\FUNK 25_KALK_NL_Reinigung_MASTER_DG_20250708.xlsx.url","lastModified":"2025-07-09T11:58:14.000Z","refIndex":42027,"score":0.000029930999877580322},{"name":"FUNK25_H12_KALK_SASSE_REINIGUNG_RW_20250917.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\Kühne + Nagel (Lager H12)\\FUNK25_H12_KALK_SASSE_REINIGUNG_RW_20250917.xlsx","lastModified":"2025-09-26T08:18:00.000Z","refIndex":42013,"score":0.000046127927499884805},{"name":"FUNK 25_KALK_NL_PK H6 3_RT_20250502 - storniert.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FUNK\\FUNK 25\\009_Reinigung und Entsorgung\\Kalkulation\\NEWLINE\\FUNK 25_KALK_NL_PK H6 3_RT_20250502 - storniert.xlsx","lastModified":"2025-08-29T13:35:26.000Z","refIndex":41986,"score":0.00006614538371855344}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"FUNK 25","base":"FUNK","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>INTER</t>
+  </si>
+  <si>
+    <t>[{"name":"INTER1197_KALK_SASSE_REINIGUNG_RW_20250320.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1197\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1197_KALK_SASSE_REINIGUNG_RW_20250320.xlsx","lastModified":"2025-04-02T11:50:49.000Z","refIndex":308,"score":0.0000028750131789367335},{"name":"INTER1201_KAL_SASSE_Reinigung_DG_20250606.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1201\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1201_KAL_SASSE_Reinigung_DG_20250606.xlsx","lastModified":"2025-06-06T08:07:02.000Z","refIndex":310,"score":0.0000028750131789367335},{"name":"INTER1201_KAL_SASSE_Reinigung_DG_20250606_neu.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1201\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1201_KAL_SASSE_Reinigung_DG_20250606_neu.xlsx","lastModified":"2025-06-06T09:49:10.000Z","refIndex":311,"score":0.0000028750131789367335},{"name":"INTER1203_KAL_SASSE_Reinigung_RW_20250627.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1203\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1203_KAL_SASSE_Reinigung_RW_20250627.xlsx","lastModified":"2025-07-30T10:55:13.000Z","refIndex":316,"score":0.0000028750131789367335},{"name":"INTER1206_ABR_SASSE_Reinigung_DG_20250602.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1206\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1206_ABR_SASSE_Reinigung_DG_20250602.xlsx","lastModified":"2025-06-02T12:09:49.000Z","refIndex":330,"score":0.0000028750131789367335},{"name":"INTER1206_KAL_SASSE_Reinigung_DG_20250509.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1206\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1206_KAL_SASSE_Reinigung_DG_20250509.xlsx","lastModified":"2025-05-09T10:12:01.000Z","refIndex":331,"score":0.0000028750131789367335},{"name":"INTER-MB-Frühlingsfest_KALK_SASSE_REINIGUNG_RW_20250320.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1208\\009_Reinigung und Entsorgung\\Kalkulation\\INTER-MB-Frühlingsfest_KALK_SASSE_REINIGUNG_RW_20250320.xlsx","lastModified":"2025-04-25T04:40:16.000Z","refIndex":334,"score":0.0000028750131789367335},{"name":"INTER1210_KALK_SASSE_REINIGUNG_RW_20250228.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1210\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1210_KALK_SASSE_REINIGUNG_RW_20250228.xlsx","lastModified":"2025-04-02T11:41:43.000Z","refIndex":358,"score":0.0000028750131789367335},{"name":"INTER1212_Rest_BRB_ABR_WISAG_Reinigung_VM_20250224.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1212\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1212_Rest_BRB_ABR_WISAG_Reinigung_VM_20250224.xlsx","lastModified":"2025-03-24T09:32:13.000Z","refIndex":376,"score":0.0000028750131789367335},{"name":"INTER1212_Rest_BRB_KALK_WISAG_Reinigung_JI_20250215.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1212\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1212_Rest_BRB_KALK_WISAG_Reinigung_JI_20250215.xlsx","lastModified":"2025-02-25T06:45:47.000Z","refIndex":377,"score":0.0000028750131789367335},{"name":"INTER1214_KALK_SASSE_Reinigung_DG_20250619.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1214\\009_Reinigung und Entsorgung\\Kalkulation\\INTER1214_KALK_SASSE_Reinigung_DG_20250619.xlsx","lastModified":"2025-06-23T18:59:50.000Z","refIndex":386,"score":0.0000028750131789367335},{"name":"INTER 1202_BECC_KALK_SASSE_Reinigung_RT_20250821.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\INTER\\INTER1202\\009_Reinigung und Entsorgung\\Kalkulation\\INTER 1202_BECC_KALK_SASSE_Reinigung_RT_20250821.xlsx","lastModified":"2025-09-08T10:21:04.000Z","refIndex":314,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1235","base":"INTER","number":"1235","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1202","base":"INTER","number":"1202","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>IHK</t>
+  </si>
+  <si>
+    <t>[{"name":"IHK25-2_KALK_CWS_Ladycare_DG_20250313.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\IHK25-2_KALK_CWS_Ladycare_DG_20250313.xlsx","lastModified":"2025-03-13T11:23:28.000Z","refIndex":737,"score":0.000006128646825844065},{"name":"IHK25-2_ABR_SASSE_Reinigung_NK_20250410.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\SASSE\\IHK25-2_ABR_SASSE_Reinigung_NK_20250410.xlsx","lastModified":"2025-04-10T11:39:22.000Z","refIndex":742,"score":0.000006128646825844065},{"name":"IHK25-2_BECC_SASSE_Reinigung_DG_20250312.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\SASSE\\IHK25-2_BECC_SASSE_Reinigung_DG_20250312.xlsx","lastModified":"2025-03-13T10:56:39.000Z","refIndex":743,"score":0.000006128646825844065},{"name":"IHK 25 2_BECC_ALBA_Entsorgung_RT_20250305.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\IHK 25 2_BECC_ALBA_Entsorgung_RT_20250305.xlsx","lastModified":"2025-03-05T11:13:26.000Z","refIndex":734,"score":0.000018733759825364087},{"name":"IHK 25 2_BECC_ABR_NEWLINE_Reinigung_DS_20250326.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\IHK 25 2_BECC_ABR_NEWLINE_Reinigung_DS_20250326.xlsx","lastModified":"2025-03-26T11:13:37.000Z","refIndex":738,"score":0.000018733759825364087},{"name":"IHK 25 2_BECC_NEWLINE_Reinigung_DG_20250313.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\IHK 25 2_BECC_NEWLINE_Reinigung_DG_20250313.xlsx","lastModified":"2025-03-13T15:57:48.000Z","refIndex":739,"score":0.000018733759825364087},{"name":"IHK 25 2_KALK_NL_Reinigung_DG_20250314.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\2\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\IHK 25 2_KALK_NL_Reinigung_DG_20250314.xlsx","lastModified":"2025-03-25T10:32:21.000Z","refIndex":741,"score":0.000018733759825364087},{"name":"IHK 25 3_SASSE_Reinigung_NK_20250718.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\3\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 3_SASSE_Reinigung_NK_20250718.xlsx","lastModified":"2025-07-18T10:08:11.000Z","refIndex":773,"score":0.000018733759825364087},{"name":"IHK 25 3_SASSE_Reinigung_RT_20250619.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\3\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 3_SASSE_Reinigung_RT_20250619.xlsx","lastModified":"2025-06-19T08:47:20.000Z","refIndex":774,"score":0.000018733759825364087},{"name":"IHK 25 4_ALBA_Entsorgung_RT_20250416.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_ALBA_Entsorgung_RT_20250416.xlsx","lastModified":"2025-04-16T07:19:42.000Z","refIndex":811,"score":0.000018733759825364087},{"name":"IHK 25 4_NEWLINE_Reinigung_RT_20250423.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_NEWLINE_Reinigung_RT_20250423.xlsx","lastModified":"2025-04-23T05:03:34.000Z","refIndex":816,"score":0.000018733759825364087},{"name":"IHK 25 4_SASSE_Reinigung_RT_20250423.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_SASSE_Reinigung_RT_20250423.xlsx","lastModified":"2025-04-23T04:54:41.000Z","refIndex":817,"score":0.000018733759825364087},{"name":"IHK 25 4_WISAG_Abrechnung_VM_20250513.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_WISAG_Abrechnung_VM_20250513.xlsx","lastModified":"2025-05-13T10:43:41.035Z","refIndex":818,"score":0.000018733759825364087},{"name":"IHK 25 4_WISAG_Reinigung_RT_20250416.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_WISAG_Reinigung_RT_20250416.xlsx","lastModified":"2025-04-16T07:39:28.000Z","refIndex":820,"score":0.000018733759825364087},{"name":"IHK 25 5_KALK_CWS_WC-Planung_RT_20250805.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\5\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 5_KALK_CWS_WC-Planung_RT_20250805.xlsx","lastModified":"2025-08-05T09:32:18.000Z","refIndex":869,"score":0.000018733759825364087},{"name":"IHK 25 5_KALK_SASSE_Reinigung_RT_20250805.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\5\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 5_KALK_SASSE_Reinigung_RT_20250805.xlsx","lastModified":"2025-08-05T10:57:06.000Z","refIndex":870,"score":0.000018733759825364087},{"name":"IHK 25 4_CWS_WC Planung_RT_20250425.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\IHK 25 4_CWS_WC Planung_RT_20250425.xlsx","lastModified":"2025-04-28T06:08:21.000Z","refIndex":814,"score":0.000029930999877580322},{"name":"Projektabrechnung  IHK Mai 2025.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\IHK\\IHK 25\\4\\009_Reinigung und Entsorgung\\Kalkulation\\Projektabrechnung  IHK Mai 2025.xlsx","lastModified":"2025-05-22T08:52:10.000Z","refIndex":822,"score":0.000029930999877580322}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"IHK 25/5","base":"IHK","number":"25/5","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1227","base":"INTER","number":"1227","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>[{"name":"CMS25_FREI_ALBA_Abrechnung_Kehrmaschinen_ES_DG_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Bestellungen\\ALBA\\CMS25_FREI_ALBA_Abrechnung_Kehrmaschinen_ES_DG_20250926.xlsx","lastModified":"2025-09-26T16:08:39.000Z","refIndex":2925,"score":0.000006128646825844065},{"name":"CMS25_ABR_ALBA_Entsorgung_DG_20251006.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\CMS25_ABR_ALBA_Entsorgung_DG_20251006.xlsx","lastModified":"2025-10-06T14:14:13.000Z","refIndex":2941,"score":0.000006128646825844065},{"name":"CMS25_KAL_ALBA_Abfallentsorgung_DG_20250907.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\CMS25_KAL_ALBA_Abfallentsorgung_DG_20250907.xlsx","lastModified":"2025-09-12T12:49:04.000Z","refIndex":2942,"score":0.000006128646825844065},{"name":"CMS25_KAL_ALBA_Kehrmaschine_DG_20250912.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\CMS25_KAL_ALBA_Kehrmaschine_DG_20250912.xlsx","lastModified":"2025-09-12T12:03:19.000Z","refIndex":2943,"score":0.000006128646825844065},{"name":"CMS25_CWS_Kostenplanung_Schmutzfangmatten_DG_20250908dg.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\CMS25_CWS_Kostenplanung_Schmutzfangmatten_DG_20250908dg.xlsx","lastModified":"2025-09-08T15:48:59.000Z","refIndex":2944,"score":0.000006128646825844065},{"name":"CMS25_KALK_NL_Reinigung_DG_20250915.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\CMS25_KALK_NL_Reinigung_DG_20250915.xlsx","lastModified":"2025-09-18T09:04:12.000Z","refIndex":2947,"score":0.000006128646825844065},{"name":"CMS25_KALK_NL_Reinigung_DG_20250918.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\CMS25_KALK_NL_Reinigung_DG_20250918.xlsx","lastModified":"2025-09-18T15:14:26.000Z","refIndex":2948,"score":0.000006128646825844065},{"name":"CMS25_KALK_NL_Reinigung_DG_20250922.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\CMS25_KALK_NL_Reinigung_DG_20250922.xlsx","lastModified":"2025-09-22T15:27:56.000Z","refIndex":2949,"score":0.000006128646825844065},{"name":"CMS25_KAL_SASSE_Reinigung_RW_20250924.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\SASSE\\CMS25_KAL_SASSE_Reinigung_RW_20250924.xlsx","lastModified":"2025-09-24T08:36:15.000Z","refIndex":2950,"score":0.000006128646825844065},{"name":"CMS25_Ideelle-Stände_DG_20250908.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\ideelle Flächen\\CMS25_Ideelle-Stände_DG_20250908.xlsx","lastModified":"2025-09-08T10:01:12.000Z","refIndex":2938,"score":0.00001131032569734829},{"name":"CMS25_BECC_KAL_WISAG_Glas-Reinigung_DG_20250907.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG Glas\\CMS25_BECC_KAL_WISAG_Glas-Reinigung_DG_20250907.xlsx","lastModified":"2025-09-30T04:53:35.000Z","refIndex":2951,"score":0.00001131032569734829},{"name":"GewerkezeitplanCMS25_vogez. Aufbauzeiten 19_08_2025.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\Veranstaltungsinfo\\GewerkezeitplanCMS25_vogez. Aufbauzeiten 19_08_2025.xlsx","lastModified":"2025-08-22T06:26:38.000Z","refIndex":2958,"score":0.000018733759825364087},{"name":"CMS25_BECC_KAL_WISAG_Glas-Reinigung_DG_20250907.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\MBProProd\\CMS 25 - Reinigung u. Entsorgung ES\\CMS25_BECC_KAL_WISAG_Glas-Reinigung_DG_20250907.xlsx","lastModified":"2025-09-11T12:35:51.000Z","refIndex":2952,"score":0.0000914916749118376},{"name":"CMS25_KALK_NL_Reinigung_DG_20250918.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\MBProProd\\CMS 25 - Reinigung u. Entsorgung ES\\CMS25_KALK_NL_Reinigung_DG_20250918.xlsx","lastModified":"2025-09-18T15:15:04.000Z","refIndex":2953,"score":0.0000914916749118376},{"name":"CMS25_KAL_ALBA_Abfallentsorgung_DG_20250907.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\MBProProd\\CMS 25 - Reinigung u. Entsorgung ES\\CMS25_KAL_ALBA_Abfallentsorgung_DG_20250907.xlsx","lastModified":"2025-09-12T13:01:35.000Z","refIndex":2954,"score":0.0000914916749118376},{"name":"CMS25_KAL_SASSE_Reinigung_RW_20250924.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\CMS\\CMS 25\\009_Reinigung und Entsorgung\\MBProProd\\CMS 25 - Reinigung u. Entsorgung ES\\CMS25_KAL_SASSE_Reinigung_RW_20250924.xlsx","lastModified":"2025-09-24T08:57:41.000Z","refIndex":2955,"score":0.0000914916749118376}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"CMS 25","base":"CMS","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>DROID</t>
+  </si>
+  <si>
+    <t>[{"name":"DROID25_KALK_SASSE_Reinigung_DG_20250910.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25\\009_Reinigung und Entsorgung\\Kalkulation\\DROID25_KALK_SASSE_Reinigung_DG_20250910.xlsx","lastModified":"2025-09-16T09:00:11.000Z","refIndex":434,"score":0.000006128646825844065},{"name":"DROID25_KALK_SASSE_Reinigung_RT_20250916.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25\\009_Reinigung und Entsorgung\\Kalkulation\\DROID25_KALK_SASSE_Reinigung_RT_20250916.xlsx","lastModified":"2025-09-22T08:40:07.000Z","refIndex":435,"score":0.000006128646825844065},{"name":"DROID25_KALK_SASSE_Reinigung_RT_20250924.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25\\009_Reinigung und Entsorgung\\Kalkulation\\DROID25_KALK_SASSE_Reinigung_RT_20250924.xlsx","lastModified":"2025-09-24T05:59:48.294Z","refIndex":436,"score":0.000006128646825844065},{"name":"DROID25_ABR_ALBA_Abfallentsorgung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25A\\009_Reinigung und Entsorgung\\Kalkulation\\DROID25_ABR_ALBA_Abfallentsorgung_DG_20251001.xlsx","lastModified":"2025-10-01T10:09:56.000Z","refIndex":527,"score":0.000006128646825844065},{"name":"DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25\\009_Reinigung und Entsorgung\\Kalkulation\\DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx","lastModified":"2025-09-10T12:35:42.000Z","refIndex":432,"score":0.00001131032569734829},{"name":"DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DROID\\DROID 25A - nicht benutzen\\009_Reinigung und Entsorgung\\Kalkulation\\DROID 25_KALK_ALBA_Reinigung_RT_20250523.xlsx","lastModified":"2025-09-10T12:37:12.000Z","refIndex":601,"score":0.000046127927499884805}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"DROID 25A","base":"DROID","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>VENUS</t>
+  </si>
+  <si>
+    <t>[{"name":"VENUS25_BECC_ABR_ALBA_Entsorgung_ET_20251003.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VENUS\\VENUS 25\\009_Reinigung und Entsorgung\\Kalkulation\\VENUS25_BECC_ABR_ALBA_Entsorgung_ET_20251003.xlsx","lastModified":"2025-10-03T08:12:42.000Z","refIndex":1234,"score":0.000006128646825844065},{"name":"VENUS25_BECC_ABR_WISAG_Reinigung_VM_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VENUS\\VENUS 25\\009_Reinigung und Entsorgung\\Kalkulation\\VENUS25_BECC_ABR_WISAG_Reinigung_VM_20251001.xlsx","lastModified":"2025-10-02T06:30:07.000Z","refIndex":1235,"score":0.000006128646825844065},{"name":"VENUS25_BECC_KAL_ALBA_Entsorgung_JI_20250919.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VENUS\\VENUS 25\\009_Reinigung und Entsorgung\\Kalkulation\\VENUS25_BECC_KAL_ALBA_Entsorgung_JI_20250919.xlsx","lastModified":"2025-09-19T12:29:47.000Z","refIndex":1237,"score":0.000006128646825844065},{"name":"VENUS25_BECC_KAL_WISAG_Reinigung_JI_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VENUS\\VENUS 25\\009_Reinigung und Entsorgung\\Kalkulation\\VENUS25_BECC_KAL_WISAG_Reinigung_JI_20251001.xlsx","lastModified":"2025-10-01T10:01:30.000Z","refIndex":1238,"score":0.000006128646825844065},{"name":"VENUS25_BECC_KAL_WISAG_Reinigung_RW_20250923.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VENUS\\VENUS 25\\009_Reinigung und Entsorgung\\Kalkulation\\VENUS25_BECC_KAL_WISAG_Reinigung_RW_20250923.xlsx","lastModified":"2025-09-23T08:48:45.000Z","refIndex":1239,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"VENUS 25","base":"VENUS","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>STUZUBI</t>
+  </si>
+  <si>
+    <t>[{"name":"STUZUBI25_H21_ABR_ALBA_Entsorgung_DG_20250224.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25_H21_ABR_ALBA_Entsorgung_DG_20250224.xlsx","lastModified":"2025-09-06T11:05:25.000Z","refIndex":163,"score":0.000006128646825844065},{"name":"STUZUBI25_H21_ABR_WISAG_Reinigung_VM_20250218.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25_H21_ABR_WISAG_Reinigung_VM_20250218.xlsx","lastModified":"2025-09-06T06:56:38.000Z","refIndex":166,"score":0.000006128646825844065},{"name":"STUZUBI25_H21_KAL_ALBA_Entsorgung_Forecast_JI_20250207.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25_H21_KAL_ALBA_Entsorgung_Forecast_JI_20250207.xlsx","lastModified":"2025-02-07T11:27:40.000Z","refIndex":171,"score":0.000006128646825844065},{"name":"STUZUBI25_H21_KAL_WISAG_Reinigung_JI_20250206.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25_H21_KAL_WISAG_Reinigung_JI_20250206.xlsx","lastModified":"2025-02-07T10:57:05.000Z","refIndex":174,"score":0.000006128646825844065},{"name":"STUZUBI25_H21_KAL_ALBA_Entsorgung_Forecast_JI_20250207.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\MBPro\\Dev\\Entsorgung\\STUZUBI25_H21_KAL_ALBA_Entsorgung_Forecast_JI_20250207.xlsx","lastModified":"2025-02-07T11:27:40.000Z","refIndex":175,"score":0.000006128646825844065},{"name":"STUZUBI25A_BECC_KAL_Alba_Entsorgung_JI_20250906.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25A\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25A_BECC_KAL_Alba_Entsorgung_JI_20250906.xlsx","lastModified":"2025-09-06T11:07:29.000Z","refIndex":258,"score":0.000006128646825844065},{"name":"STUZUBI25A_BECC_KAL_Sasse_Reinigung_JI_20250909.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25A\\009_Reinigung und Entsorgung\\Kalkulation\\STUZUBI25A_BECC_KAL_Sasse_Reinigung_JI_20250909.xlsx","lastModified":"2025-09-19T10:16:11.000Z","refIndex":259,"score":0.000006128646825844065},{"name":"STUZUBI25_H21_KAL_WISAG_Reinigung_JI_20250206.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STUZUBI\\STUZUBI 25\\009_Reinigung und Entsorgung\\MBPro\\Entwurf Reinigungslayout Febr. VA 2025\\STUZUBI25_H21_KAL_WISAG_Reinigung_JI_20250206.xlsx","lastModified":"2025-02-07T10:57:05.000Z","refIndex":179,"score":0.000046127927499884805}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"STUZUBI25A","base":"STUZUBI","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>SCC</t>
+  </si>
+  <si>
+    <t>[{"name":"SCC25_BECC_KAL_Alba_Entsorgung_JI_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SCC\\SCC 25\\009_Reinigung und Entsorgung\\Kalkulation\\Alba\\SCC25_BECC_KAL_Alba_Entsorgung_JI_20250926.xlsx","lastModified":"2025-09-26T07:28:43.000Z","refIndex":4129,"score":0.000006128646825844065},{"name":"SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SCC\\SCC 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","lastModified":"2025-10-01T05:46:51.000Z","refIndex":4134,"score":0.000006128646825844065},{"name":"SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SCC\\SCC 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG GLAS\\SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","lastModified":"2025-08-21T09:11:08.000Z","refIndex":4137,"score":0.00001131032569734829},{"name":"SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SCC\\SCC 25\\009_Reinigung und Entsorgung\\MBPro\\Prod\\Reinigung und Entsorgung Smart Country Convention 2025\\SCC25_BECC_KAL_WISAG_Reinigung_JI_20250821.xlsx","lastModified":"2025-09-11T11:09:38.000Z","refIndex":4138,"score":0.0000914916749118376}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"SCC 25","base":"SCC","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>FILM</t>
+  </si>
+  <si>
+    <t>[{"name":"FILM496_KAL_WC_Planung_DG_20250929.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FILM\\FILM 496\\009_Reinigung und Entsorgung\\Bestellungen\\FILM496_KAL_WC_Planung_DG_20250929.xlsx","lastModified":"2025-09-29T10:51:34.000Z","refIndex":126,"score":0.000006128646825844065},{"name":"FILM496_KAL_ALBA_Entsorgung_DG_20251003.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FILM\\FILM 496\\009_Reinigung und Entsorgung\\Kalkulation\\FILM496_KAL_ALBA_Entsorgung_DG_20251003.xlsx","lastModified":"2025-10-03T09:25:14.000Z","refIndex":127,"score":0.000006128646825844065},{"name":"FILM496_KAL_NL_Reinigung_DG_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FILM\\FILM 496\\009_Reinigung und Entsorgung\\Kalkulation\\FILM496_KAL_NL_Reinigung_DG_20250926.xlsx","lastModified":"2025-09-26T12:14:38.000Z","refIndex":128,"score":0.000006128646825844065},{"name":"FILM496_KAL_NL_Reinigung_DG_20251002.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\FILM\\FILM 496\\009_Reinigung und Entsorgung\\Kalkulation\\FILM496_KAL_NL_Reinigung_DG_20251002.xlsx","lastModified":"2025-10-02T09:31:43.000Z","refIndex":129,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"FILM 496","base":"FILM","number":"496","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>UEGW</t>
+  </si>
+  <si>
+    <t>[{"name":"UEGW25_KALK_NEWLINE_REINIGUNG_DG_20251004.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\Kalkulation\\NewLine\\UEGW25_KALK_NEWLINE_REINIGUNG_DG_20251004.xlsx","lastModified":"2025-10-07T06:43:47.000Z","refIndex":732,"score":0.000006128646825844065},{"name":"UEGW25_KALK_SASSE_REINIGUNG_RW_20251004.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\UEGW25_KALK_SASSE_REINIGUNG_RW_20251004.xlsx","lastModified":"2025-10-07T06:15:18.000Z","refIndex":733,"score":0.000006128646825844065},{"name":"UEGW25_KALK_NEWLINE_REINIGUNG_RW_20250716.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\MBPro\\UEGW25_KALK_NEWLINE_REINIGUNG_RW_20250716.xlsx","lastModified":"2025-07-16T04:49:21.000Z","refIndex":738,"score":0.000006128646825844065},{"name":"UEGW25_KALK_SASSE_REINIGUNG_RW_20250716.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\MBPro\\UEGW25_KALK_SASSE_REINIGUNG_RW_20250716.xlsx","lastModified":"2025-07-16T04:42:19.000Z","refIndex":739,"score":0.000006128646825844065},{"name":"UEGW25_KALK_WISAG_GLAS_RW_20250604.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\MBPro\\UEGW25_KALK_WISAG_GLAS_RW_20250604.xlsx","lastModified":"2025-07-16T04:49:10.000Z","refIndex":740,"score":0.000006128646825844065},{"name":"UEGWeek2025_Berlin_Master_Raumbelegungsplan.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\UEGWeek2025_Berlin_Master_Raumbelegungsplan.xlsx","lastModified":"2025-06-03T17:46:07.000Z","refIndex":744,"score":0.000006128646825844065},{"name":"UEGW25_KALK_CWS_MATTEN_RW_20250717.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS Schmutzfangmatten\\UEGW25_KALK_CWS_MATTEN_RW_20250717.xlsx","lastModified":"2025-10-01T05:06:00.000Z","refIndex":731,"score":0.00001131032569734829},{"name":"UEGW25_KALK_WISAG_GLAS_RW_20250604.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\Kalkulation\\Wisag Glas\\UEGW25_KALK_WISAG_GLAS_RW_20250604.xlsx","lastModified":"2025-06-05T07:26:20.000Z","refIndex":737,"score":0.00001131032569734829},{"name":"UEGW 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UEGW\\UEGW 25\\009_Reinigung und Entsorgung\\UEGW 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","lastModified":"2025-10-02T07:22:38.000Z","refIndex":743,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"UEGW 25","base":"UEGW","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>BCB</t>
+  </si>
+  <si>
+    <t>[{"name":"BCB25_BECC_KAL_Alba_Entsorgung_JI_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\Alba\\BCB25_BECC_KAL_Alba_Entsorgung_JI_20250926.xlsx","lastModified":"2025-09-30T11:41:18.000Z","refIndex":1982,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_Alba_WasteServices_CA_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\Alba\\BCB25_BECC_KAL_Alba_WasteServices_CA_20250930.xlsx","lastModified":"2025-10-01T07:07:53.000Z","refIndex":1983,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_Alba_WasteServices_JI_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\Alba\\BCB25_BECC_KAL_Alba_WasteServices_JI_20250926.xlsx","lastModified":"2025-09-26T10:07:15.000Z","refIndex":1984,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_CWS_Ladycare_JI_20250915.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\BCB25_BECC_KAL_CWS_Ladycare_JI_20250915.xlsx","lastModified":"2025-10-02T09:59:07.000Z","refIndex":1986,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_Sasse_Reinigung_JI_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\BCB25_BECC_KAL_Sasse_Reinigung_JI_20250930.xlsx","lastModified":"2025-10-01T10:58:52.000Z","refIndex":1989,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_Sasse_Reinigung_JI_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\BCB25_BECC_KAL_Sasse_Reinigung_JI_20251001.xlsx","lastModified":"2025-10-06T13:59:38.000Z","refIndex":1990,"score":0.000006128646825844065},{"name":"BCB25_BECC_KAL_WISAG_Reinigung_JI_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\BCB25_BECC_KAL_WISAG_Reinigung_JI_20250930.xlsx","lastModified":"2025-10-06T08:55:21.000Z","refIndex":1993,"score":0.000006128646825844065},{"name":"BCB 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BCB\\BCB 25\\009_Reinigung und Entsorgung\\BCB 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","lastModified":"2025-10-02T07:28:20.000Z","refIndex":1980,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"BCB 25","base":"BCB","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>STBK</t>
+  </si>
+  <si>
+    <t>[{"name":"STBK 25_KALK_SASSE_Reinigung_RT_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STBK\\STBK 25\\009_Reinigung und Entsorgung\\Kalkulation\\STBK 25_KALK_SASSE_Reinigung_RT_20250926.xlsx","lastModified":"2025-10-02T07:35:43.000Z","refIndex":124,"score":0.00001131032569734829},{"name":"STBK 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STBK\\STBK 25\\009_Reinigung und Entsorgung\\STBK 25_ES-TO-CDS_Checkliste_RT_20251002.xlsx","lastModified":"2025-10-02T07:41:56.000Z","refIndex":126,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"STBK 25","base":"STBK","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1231","base":"INTER","number":"1231","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>VAGED</t>
+  </si>
+  <si>
+    <t>[{"name":"VAGED25_BECC_KAL_Sasse_Reinigung_JI_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VAGED\\VAGED 25B\\009_Reinigung und Entsorgung\\Kalkulation\\VAGED25_BECC_KAL_Sasse_Reinigung_JI_20251007.xlsx","lastModified":"2025-10-07T07:27:46.000Z","refIndex":153,"score":0.000006128646825844065},{"name":"VAGED25_BECC_KAL_WISAG_Reinigung_JI_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VAGED\\VAGED 25B\\009_Reinigung und Entsorgung\\Kalkulation\\VAGED25_BECC_KAL_WISAG_Reinigung_JI_20251007.xlsx","lastModified":"2025-10-07T10:01:22.000Z","refIndex":154,"score":0.000006128646825844065},{"name":"250825_Übersicht_Stände_ECE2025_Standreinigung.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\VAGED\\VAGED 25B\\009_Reinigung und Entsorgung\\Veranstaltungsinfo\\250825_Übersicht_Stände_ECE2025_Standreinigung.xlsx","lastModified":"2025-08-28T09:01:33.000Z","refIndex":155,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"VAGED 25B","base":"VAGED","number":"25","ext":"B","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1236","base":"INTER","number":"1236","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>STEX</t>
+  </si>
+  <si>
+    <t>[{"name":"STEX 25_ABR_ALBA_Entsorgung_RT_20250512.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25_ABR_ALBA_Entsorgung_RT_20250512.xlsx","lastModified":"2025-05-08T11:26:56.000Z","refIndex":720,"score":0.00001131032569734829},{"name":"STEX 25_BECC_ALBA_Entsorgung_RT_20250304.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25_BECC_ALBA_Entsorgung_RT_20250304.xlsx","lastModified":"2025-03-05T07:52:03.000Z","refIndex":721,"score":0.00001131032569734829},{"name":"STEX 25_BECC_CWS_WC-Planung_RT_20250303.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25_BECC_CWS_WC-Planung_RT_20250303.xlsx","lastModified":"2025-03-05T07:52:41.000Z","refIndex":723,"score":0.00001131032569734829},{"name":"STEX 25_BECC_SASSE_Reinigung_RT_20250325.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25_BECC_SASSE_Reinigung_RT_20250325.xlsx","lastModified":"2025-03-25T08:36:13.000Z","refIndex":724,"score":0.00001131032569734829},{"name":"STEX 25_BECC_SASSE_Reinigung_RT_20250414.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25_BECC_SASSE_Reinigung_RT_20250414.xlsx","lastModified":"2025-05-07T09:22:18.000Z","refIndex":725,"score":0.00001131032569734829},{"name":"STEX 25A_BECC_KAL_CWS_WC-Planung_RT_20250811.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25A\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25A_BECC_KAL_CWS_WC-Planung_RT_20250811.xlsx","lastModified":"2025-08-11T08:11:28.000Z","refIndex":741,"score":0.00001131032569734829},{"name":"STEX 25A_BECC_KAL_WISAG_Reinigung_RT_20250926.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\STEX\\STEX 25A\\009_Reinigung und Entsorgung\\Kalkulation\\STEX 25A_BECC_KAL_WISAG_Reinigung_RT_20250926.xlsx","lastModified":"2025-09-26T06:11:06.000Z","refIndex":742,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"STEX 25A","base":"STEX","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>ESMO</t>
+  </si>
+  <si>
+    <t>[{"name":"ESMO25_KALK_NEWLINE_REINIGUNG_MASTER_2025_10_07.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Kalkulation\\NewLine\\ESMO25_KALK_NEWLINE_REINIGUNG_MASTER_2025_10_07.xlsx","lastModified":"2025-10-07T09:58:30.000Z","refIndex":818,"score":0.000006128646825844065},{"name":"ESMO25_KALK_SASSE_REINIGUNG_MASTER_RW_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Kalkulation\\Sasse\\ESMO25_KALK_SASSE_REINIGUNG_MASTER_RW_20251007.xlsx","lastModified":"2025-10-07T08:33:09.000Z","refIndex":819,"score":0.000006128646825844065},{"name":"ESMO25_BECC_KAL_WISAG_Reinigung_MASTER_RW_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Kalkulation\\Wisag\\ESMO25_BECC_KAL_WISAG_Reinigung_MASTER_RW_20251007.xlsx","lastModified":"2025-10-07T08:34:10.000Z","refIndex":825,"score":0.000006128646825844065},{"name":"ESMO25_KALK_NEWLINE_REINIGUNG_MASTER_2025.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\MBPro\\Prod\\NewLine\\ESMO25_KALK_NEWLINE_REINIGUNG_MASTER_2025.xlsx.url","lastModified":"2025-08-06T12:54:36.000Z","refIndex":827,"score":0.000006128646825844065},{"name":"ESMO25_KALK_SASSE_REINIGUNG_MASTER_RW_20250722.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\MBPro\\Prod\\Sasse\\ESMO25_KALK_SASSE_REINIGUNG_MASTER_RW_20250722.xlsx.url","lastModified":"2025-08-06T13:07:31.000Z","refIndex":828,"score":0.000006128646825844065},{"name":"ESMO25_BECC_KAL_WISAG_Reinigung_MASTER_RW_20250722.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\MBPro\\Prod\\Wisag\\ESMO25_BECC_KAL_WISAG_Reinigung_MASTER_RW_20250722.xlsx.url","lastModified":"2025-08-06T13:08:22.000Z","refIndex":829,"score":0.000006128646825844065},{"name":"ESMO25_BECC_KAL_CWS_WC-Planung_MASTER_RW_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Kalkulation\\CWS (Ladycare)\\ESMO25_BECC_KAL_CWS_WC-Planung_MASTER_RW_20251007.xlsx","lastModified":"2025-10-07T08:34:13.000Z","refIndex":817,"score":0.00001131032569734829},{"name":"ESMO25_KALK_WISAG_Glasreinigung_RW_20250328.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Kalkulation\\Wisag Glas\\ESMO25_KALK_WISAG_Glasreinigung_RW_20250328.xlsx","lastModified":"2025-09-26T06:13:47.000Z","refIndex":826,"score":0.00001131032569734829},{"name":"ESMO25_KALK_WISAG_Glasreinigung_RW_20250328.xlsx.url","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\MBPro\\Prod\\Wisag Glas\\ESMO25_KALK_WISAG_Glasreinigung_RW_20250328.xlsx.url","lastModified":"2025-08-06T13:14:38.000Z","refIndex":830,"score":0.00001131032569734829},{"name":"DRK-Stationen First_Aid_planning_2025_05_27.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\Veranstaltungsinfo\\DRK-Stationen First_Aid_planning_2025_05_27.xlsx","lastModified":"2025-05-28T14:30:08.000Z","refIndex":833,"score":0.00001131032569734829},{"name":"ESMO 2025_Cleaning overview_250731.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ESMO\\ESMO 25A\\009_Reinigung und Entsorgung\\ESMO 2025_Cleaning overview_250731.xlsx","lastModified":"2025-08-04T13:21:43.000Z","refIndex":813,"score":0.000018733759825364087}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"ESMO 25A","base":"ESMO","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>ANIMACO</t>
+  </si>
+  <si>
+    <t>[{"name":"ANIMACO 25_BECC_ES-TO-CDS_Checkliste_RT_20250902.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ANIMACO\\ANIMACO 25\\009_Reinigung und Entsorgung\\ANIMACO 25_BECC_ES-TO-CDS_Checkliste_RT_20250902.xlsx","lastModified":"2025-09-03T05:14:50.000Z","refIndex":603,"score":0.00001131032569734829},{"name":"ANIMACO 25_KALK_SASSE_Reinigung_RT_20250805.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\ANIMACO\\ANIMACO 25\\009_Reinigung und Entsorgung\\Kalkulation\\ANIMACO 25_KALK_SASSE_Reinigung_RT_20250805.xlsx","lastModified":"2025-09-30T08:23:23.000Z","refIndex":605,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"ANIMACO 25","base":"ANIMACO","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>UNFALL</t>
+  </si>
+  <si>
+    <t>[{"name":"UNFALL 25A_KALK_ALBA_Entsorgung_RT_20250806.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UNFALL\\UNFALL25A\\009_Reinigung und Entsorgung\\Kalkulation\\UNFALL 25A_KALK_ALBA_Entsorgung_RT_20250806.xlsx","lastModified":"2025-09-24T14:20:59.000Z","refIndex":2012,"score":0.000006128646825844065},{"name":"UNFALL 25A_KALK_SASSE_Reinigung_DG_20250911.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UNFALL\\UNFALL25A\\009_Reinigung und Entsorgung\\Kalkulation\\UNFALL 25A_KALK_SASSE_Reinigung_DG_20250911.xlsx","lastModified":"2025-10-06T07:21:14.000Z","refIndex":2013,"score":0.000006128646825844065},{"name":"UNFALL 25A_KALK_WISAG_Glasreinigng_RT_20250925.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\UNFALL\\UNFALL25A\\009_Reinigung und Entsorgung\\Kalkulation\\UNFALL 25A_KALK_WISAG_Glasreinigng_RT_20250925.xlsx","lastModified":"2025-09-26T14:50:50.000Z","refIndex":2014,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"UNFALL25A","base":"UNFALL","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>[{"name":"SAP 25C_KALK_ALBA_Entsorgung_RT_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SAP\\SAP 25C\\009_Reinigung und Entsorgung\\Kalkulation\\SAP 25C_KALK_ALBA_Entsorgung_RT_20250930.xlsx","lastModified":"2025-09-30T05:32:07.000Z","refIndex":150,"score":0.00001131032569734829},{"name":"SAP 25C_KALK_NEWLINE_Reinigung_RT_20250929.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SAP\\SAP 25C\\009_Reinigung und Entsorgung\\Kalkulation\\SAP 25C_KALK_NEWLINE_Reinigung_RT_20250929.xlsx","lastModified":"2025-09-30T05:34:48.068Z","refIndex":151,"score":0.00001131032569734829},{"name":"SAP 25C_KALK_WISAG_Glas_RT_20250930.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SAP\\SAP 25C\\009_Reinigung und Entsorgung\\Kalkulation\\SAP 25C_KALK_WISAG_Glas_RT_20250930.xlsx","lastModified":"2025-09-30T05:09:12.567Z","refIndex":152,"score":0.00001131032569734829},{"name":"SAP 25C_KALK_WISAG_Reinigung_RT_20250929.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\SAP\\SAP 25C\\009_Reinigung und Entsorgung\\Kalkulation\\SAP 25C_KALK_WISAG_Reinigung_RT_20250929.xlsx","lastModified":"2025-09-30T04:43:12.000Z","refIndex":153,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"SAP 25C","base":"SAP","number":"25","ext":"C","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>BAZAAR</t>
+  </si>
+  <si>
+    <t>[{"name":"BAZAAR25_BECC_KAL_Sasse_Reinigung_JI_20250714.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BAZAAR\\BAZAAR 25\\009_Reinigung und Entsorgung\\Kalkulation\\BAZAAR25_BECC_KAL_Sasse_Reinigung_JI_20250714.xlsx","lastModified":"2025-10-06T09:33:45.000Z","refIndex":1528,"score":0.000006128646825844065},{"name":"BAZAAR25_BECC_KAL_Wisag_Reinigung_JI_20250714.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BAZAAR\\BAZAAR 25\\009_Reinigung und Entsorgung\\Kalkulation\\BAZAAR25_BECC_KAL_Wisag_Reinigung_JI_20250714.xlsx","lastModified":"2025-10-06T09:30:18.000Z","refIndex":1529,"score":0.000006128646825844065},{"name":"BAZAAR25_KAL_WISAG_Reinigung_DG_20251006.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BAZAAR\\BAZAAR 25\\009_Reinigung und Entsorgung\\Kalkulation\\BAZAAR25_KAL_WISAG_Reinigung_DG_20251006.xlsx","lastModified":"2025-10-06T15:25:03.000Z","refIndex":1530,"score":0.000006128646825844065},{"name":"BAZAAR26_BECC_Forecast_Sasse_Reinigung_JI_20250721.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BAZAAR\\BAZAAR 26\\009_Reinigung und Entsorgung\\Kalkulation\\BAZAAR26_BECC_Forecast_Sasse_Reinigung_JI_20250721.xlsx","lastModified":"2025-07-21T08:07:19.000Z","refIndex":1586,"score":0.000006128646825844065},{"name":"BAZAAR26_BECC_Forecast_Wisag_Reinigung_JI_20250717.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BAZAAR\\BAZAAR 26\\009_Reinigung und Entsorgung\\Kalkulation\\BAZAAR26_BECC_Forecast_Wisag_Reinigung_JI_20250717.xlsx","lastModified":"2025-07-21T08:13:06.000Z","refIndex":1587,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"BAZAAR 25","base":"BAZAAR","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>DPFLEGE</t>
+  </si>
+  <si>
+    <t>[{"name":"DPFLEGE25_BECC_KAL_WISAG_Reinigung_JI_20250928.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\DPFLEGE\\DPFLEGE25B\\009_Reinigung und Entsorgung\\Kalkulation\\DPFLEGE25_BECC_KAL_WISAG_Reinigung_JI_20250928.xlsx","lastModified":"2025-09-29T10:43:57.000Z","refIndex":699,"score":0.0000028750131789367335}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"DPFLEGE25B","base":"DPFLEGE","number":"25","ext":"B","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>HUNKEM</t>
+  </si>
+  <si>
+    <t>[{"name":"HUNKEM 25_ABR_ALBA_Entsorgung_RT_20250327.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HUNKEM\\HUNKEM 25\\009_Reinigung und Entsorgung\\Kalkulation\\HUNKEM 25_ABR_ALBA_Entsorgung_RT_20250327.xlsx","lastModified":"2025-03-27T06:25:37.000Z","refIndex":478,"score":0.00001131032569734829},{"name":"HUNKEM 25_ABR_NEWLINE_Reinigung_DS_20250324.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HUNKEM\\HUNKEM 25\\009_Reinigung und Entsorgung\\Kalkulation\\HUNKEM 25_ABR_NEWLINE_Reinigung_DS_20250324.xlsx","lastModified":"2025-03-24T11:45:58.000Z","refIndex":479,"score":0.00001131032569734829},{"name":"HUNKEM 25_BECC_ALBA_Entsorgung_RT_20250305.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HUNKEM\\HUNKEM 25\\009_Reinigung und Entsorgung\\Kalkulation\\HUNKEM 25_BECC_ALBA_Entsorgung_RT_20250305.xlsx","lastModified":"2025-03-11T08:28:29.000Z","refIndex":480,"score":0.00001131032569734829},{"name":"HUNKEM 25_BECC_CWS_WC-Planung_RT_20250303.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HUNKEM\\HUNKEM 25\\009_Reinigung und Entsorgung\\Kalkulation\\HUNKEM 25_BECC_CWS_WC-Planung_RT_20250303.xlsx","lastModified":"2025-03-03T09:41:17.000Z","refIndex":482,"score":0.00001131032569734829},{"name":"HUNKEM 25_BECC_NEWLINE_Reinigung_RT_20250306.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HUNKEM\\HUNKEM 25\\009_Reinigung und Entsorgung\\Kalkulation\\HUNKEM 25_BECC_NEWLINE_Reinigung_RT_20250306.xlsx","lastModified":"2025-03-13T16:01:21.000Z","refIndex":483,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"HUNKEM 25A","base":"HUNKEM","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>HERTHA</t>
+  </si>
+  <si>
+    <t>[{"name":"HERTHA103_ABR_ALBA_Entsorgung_DG_20250530.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA103_ABR_ALBA_Entsorgung_DG_20250530.xlsx","lastModified":"2025-05-30T15:44:01.000Z","refIndex":140,"score":0.000006128646825844065},{"name":"HERTHA103_ABR_WISAG_Reinigung_DG_20250604.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA103_ABR_WISAG_Reinigung_DG_20250604.xlsx","lastModified":"2025-06-13T05:07:47.000Z","refIndex":141,"score":0.000006128646825844065},{"name":"HERTHA103_ABR_WISG_Reinigung_DG_20250604.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA103_ABR_WISG_Reinigung_DG_20250604.xlsx","lastModified":"2025-06-04T16:17:28.000Z","refIndex":142,"score":0.000006128646825844065},{"name":"HERTHA 103_BECC_ABR_WISAG_Reinigung_VM_20250612.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 103_BECC_ABR_WISAG_Reinigung_VM_20250612.xlsx","lastModified":"2025-06-12T06:22:03.000Z","refIndex":134,"score":0.00001131032569734829},{"name":"HERTHA 103_BECC_KAL_ALBA_Entsorgung_RT_20250324.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 103_BECC_KAL_ALBA_Entsorgung_RT_20250324.xlsx","lastModified":"2025-03-24T12:57:48.000Z","refIndex":135,"score":0.00001131032569734829},{"name":"HERTHA 103_BECC_KAL_CWS_Ladycareb_RT_20250324.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 103_BECC_KAL_CWS_Ladycareb_RT_20250324.xlsx","lastModified":"2025-03-24T10:32:21.000Z","refIndex":137,"score":0.00001131032569734829},{"name":"HERTHA 103_BECC_KAL_WISAG_Reinigung_JI_20250525.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 103_BECC_KAL_WISAG_Reinigung_JI_20250525.xlsx","lastModified":"2025-05-25T09:23:05.000Z","refIndex":138,"score":0.00001131032569734829},{"name":"HERTHA 103_BECC_KAL_WISAG_Reinigung_RT_20250324.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 103\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 103_BECC_KAL_WISAG_Reinigung_RT_20250324.xlsx","lastModified":"2025-05-25T09:10:15.000Z","refIndex":139,"score":0.00001131032569734829},{"name":"HERTHA 105_BECC_KAL_WISAG_Reinigung_RT_20250925.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\HERTHA\\HERTHA 105\\009_Reinigung und Entsorgung\\Kalkulation\\HERTHA 105_BECC_KAL_WISAG_Reinigung_RT_20250925.xlsx","lastModified":"2025-09-25T08:24:46.000Z","refIndex":235,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"HERTHA105","base":"HERTHA","number":"105","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>TDTLVA</t>
+  </si>
+  <si>
+    <t>[{"name":"TDTLVA25 site visit_CCB_KALK_SASSE_REINIGUNG_RW_20250826.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\TDTLVA\\TDTLVA 25\\009_Reinigung und Entsorgung\\Kalkulation\\TDTLVA25 site visit_CCB_KALK_SASSE_REINIGUNG_RW_20250826.xlsx","lastModified":"2025-09-01T10:10:04.000Z","refIndex":7,"score":0.000018733759825364087}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"TDTLVA 25","base":"TDTLVA","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>MINERA</t>
+  </si>
+  <si>
+    <t>[{"name":"MINERA 25_KALK_SASSE_Reinigung_RT_20251007.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\MINERA\\MINERA 25\\009_Reinigung und Entsorgung\\Kalkulation\\MINERA 25_KALK_SASSE_Reinigung_RT_20251007.xlsx","lastModified":"2025-10-07T05:55:25.139Z","refIndex":250,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"MINERA25A","base":"MINERA","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>JOBMEDI</t>
+  </si>
+  <si>
+    <t>[{"name":"JOBMEDI 25_BECC_KAL_WISAG_Reinigung_RT_20250902.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\JOBMEDI\\JOBMEDI 25\\009_Reinigung und Entsorgung\\Kalkulation\\JOBMEDI 25_BECC_KAL_WISAG_Reinigung_RT_20250902.xlsx","lastModified":"2025-09-02T09:48:42.000Z","refIndex":119,"score":0.00001131032569734829}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"JOBMEDI 25","base":"JOBMEDI","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>BOOTFUN</t>
+  </si>
+  <si>
+    <t>[{"name":"BOOTFUN-ACC25_KAL_ALBA_Abfallentsorgung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\BOOTFUN-ACC25_KAL_ALBA_Abfallentsorgung_DG_20251001.xlsx","lastModified":"2025-10-01T15:59:21.000Z","refIndex":2192,"score":0.000006128646825844065},{"name":"BOOTFUN25-ACC25_PLA_CWS-LADYCARE_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\LADYCARE\\BOOTFUN25-ACC25_PLA_CWS-LADYCARE_DG_20251001.xlsx","lastModified":"2025-10-01T15:45:09.000Z","refIndex":2193,"score":0.000006128646825844065},{"name":"BOOTFUN25_PLA_CWS-SCHMUTZFANG_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\CWS\\SCHMUTZFANGMATTEN\\BOOTFUN25_PLA_CWS-SCHMUTZFANG_DG_20251001.xlsx","lastModified":"2025-10-01T11:12:03.000Z","refIndex":2196,"score":0.000006128646825844065},{"name":"BOOTFUN25_KAL_NL_Reinigung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\BOOTFUN25_KAL_NL_Reinigung_DG_20251001.xlsx","lastModified":"2025-10-01T12:45:45.000Z","refIndex":2197,"score":0.000006128646825844065},{"name":"BOOTFUN25_ACC_KAL_SASSE_REINIGUNG_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\SASSE\\BOOTFUN25_ACC_KAL_SASSE_REINIGUNG_DG_20251001.xlsx","lastModified":"2025-10-01T15:19:24.000Z","refIndex":2198,"score":0.000006128646825844065},{"name":"BOOTFUN25_MAH_KAL_SASSE_Reinigung_BOBAWARD_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\SASSE\\BOOTFUN25_MAH_KAL_SASSE_Reinigung_BOBAWARD_DG_20251001.xlsx","lastModified":"2025-10-01T15:09:21.000Z","refIndex":2199,"score":0.000006128646825844065},{"name":"BOOTFUN25-ACC25_KAL_WISAG_Reinigung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\BOOTFUN\\BOOTFUN 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\BOOTFUN25-ACC25_KAL_WISAG_Reinigung_DG_20251001.xlsx","lastModified":"2025-10-01T15:04:35.000Z","refIndex":2200,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"BOOTFUN 25","base":"BOOTFUN","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>AWB</t>
+  </si>
+  <si>
+    <t>[{"name":"AWB25_KAL_ALBA_Abfallentsorgung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\AWB\\AWB 25\\009_Reinigung und Entsorgung\\Kalkulation\\ALBA\\AWB25_KAL_ALBA_Abfallentsorgung_DG_20251001.xlsx","lastModified":"2025-10-01T16:21:51.000Z","refIndex":98,"score":0.000006128646825844065},{"name":"AWB25_KAL_NL_Reinigung_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\AWB\\AWB 25\\009_Reinigung und Entsorgung\\Kalkulation\\NL\\AWB25_KAL_NL_Reinigung_DG_20251001.xlsx","lastModified":"2025-10-01T16:51:40.000Z","refIndex":99,"score":0.000006128646825844065},{"name":"AWB25_H27_KAL_WISAG-REINIGUNG_DG_20251001.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\AWB\\AWB 25\\009_Reinigung und Entsorgung\\Kalkulation\\WISAG\\AWB25_H27_KAL_WISAG-REINIGUNG_DG_20251001.xlsx","lastModified":"2025-10-01T16:49:19.000Z","refIndex":100,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"AWB 25","base":"AWB","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1225","base":"INTER","number":"1225","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1234","base":"INTER","number":"1234","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>KELLERW</t>
+  </si>
+  <si>
+    <t>[{"name":"KELLERW25_PAF_KAL_WISAG_Reinigung_JI_20250826.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\KELLERW\\KELLERW 25\\009_Reinigung und Entsorgung\\Kalkulation\\KELLERW25_PAF_KAL_WISAG_Reinigung_JI_20250826.xlsx","lastModified":"2025-08-26T11:22:02.000Z","refIndex":59,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"KELLERW 25","base":"KELLERW","number":"25","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>WEIHN</t>
+  </si>
+  <si>
+    <t>[{"name":"WEIHN24_PAF_ABR_ALBA_ENTSORGUNG_DG_20250107.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\WEIHN\\WEIHN 24\\009_Reinigung und Entsorgung\\Kalkulation\\WEIHN24_PAF_ABR_ALBA_ENTSORGUNG_DG_20250107.xlsx","lastModified":"2025-01-07T07:32:53.000Z","refIndex":147,"score":0.000006128646825844065},{"name":"WEIHN24_PAF_ABR_WISAG_Reinigung_DG_20250106.xlsx","path":"C:\\Users\\tiedemann\\Messe Berlin GmbH\\Event Services - ES-Veranstaltungsproduktion\\WEIHN\\WEIHN 24\\009_Reinigung und Entsorgung\\Kalkulation\\WEIHN24_PAF_ABR_WISAG_Reinigung_DG_20250106.xlsx","lastModified":"2025-01-06T08:09:31.000Z","refIndex":148,"score":0.000006128646825844065}]</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"WEIHN 25A","base":"WEIHN","number":"25","ext":"A","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
+  </si>
+  <si>
+    <t>{"matchcode":{"raw":"INTER1229","base":"INTER","number":"1229","ext":"","year":2025,"shortYear":25},"filesQuery":"'25 '2025 '009_Reinigung '.xlsx"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,10 +343,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,11 +682,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,49 +704,405 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>45800.24118055556</v>
-      </c>
-      <c r="D2">
-        <v>428</v>
-      </c>
-      <c r="E2">
-        <v>0.00001131032569734829</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>45800.23957175926</v>
-      </c>
-      <c r="D3">
-        <v>429</v>
-      </c>
-      <c r="E3">
-        <v>0.00001131032569734829</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>